<commit_message>
update metadata taak (vergelijking MIM)
</commit_message>
<xml_diff>
--- a/issues/60-metadata/inventarisatie_metadata_sor.xlsx
+++ b/issues/60-metadata/inventarisatie_metadata_sor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.wiersma\Documents\disgeo-imsor\issues\60-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB665B5-C12F-4120-9CFB-AF8F0F22103E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96B50DB-EB11-4B1B-A120-D1D6898D40CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="831" xr2:uid="{A40E1B74-F992-4E2A-B94D-79E463DCBFBE}"/>
+    <workbookView xWindow="-564" yWindow="276" windowWidth="11328" windowHeight="12060" tabRatio="831" activeTab="1" xr2:uid="{A40E1B74-F992-4E2A-B94D-79E463DCBFBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Instantieniveau" sheetId="3" r:id="rId1"/>
@@ -68,6 +68,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{CBFEC0D0-2DA8-4E47-A8D9-FC8C27E339E3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+"Of dit relevant is en op welke wijze de verantwoordelijke bronhouder wordt geregistreerd, wordt later gespecificeerd. "</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C8" authorId="0" shapeId="0" xr:uid="{1966CE29-D1CC-4C92-8B77-715F87E2074D}">
       <text>
         <r>
@@ -116,7 +140,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{59F6437A-F158-4D08-A404-3C0495EDD08D}">
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{908B39A3-0D79-4AD2-AC7E-01709E40469C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Het gaat over verwijzingen naar documenten/luchtfoto's/plaatsbepalingspunten. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{59F6437A-F158-4D08-A404-3C0495EDD08D}">
       <text>
         <r>
           <rPr>
@@ -140,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{81B47250-A42E-4C85-A29A-F11946A44596}">
+    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{81B47250-A42E-4C85-A29A-F11946A44596}">
       <text>
         <r>
           <rPr>
@@ -164,7 +212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{1863180F-C074-4F49-9C4B-96B043FC5D6B}">
+    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{1863180F-C074-4F49-9C4B-96B043FC5D6B}">
       <text>
         <r>
           <rPr>
@@ -198,7 +246,104 @@
     <author>Gabriella Wiersma</author>
   </authors>
   <commentList>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{F8CEF904-778A-4069-8EAA-0384F68F231D}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{9D28C651-02AC-40E7-9970-45D792D425FB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Er is een verschil tussen 'op het niveau van een objecttype' (informatiemodelniveau), en 'over een objecttype in het model' (metamodelniveau)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{0FEEBBD0-98D5-4F6E-95A4-46A7DCA3B068}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+we kunnen altijd een tagged value "bronhouder" toevoegen. Alleen lastig wanneer er meerdere waardes mogelijk zijn, aangezien een tagged value altijd een CharacterString is. De vraag is waarvoor dit nodig is - voldoet het om een tagged value te gebruiken hier?
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{97262666-69BC-4EF9-ACFE-5E4FC2F8F68D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+mogelijk via een nieuwe tagged value (?)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{FFC75014-49E1-4551-B2B5-A6FD9D783318}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+via mim:populatie tagged value (niet direct beschreven in MIM doc, wel in het diagram)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{F8CEF904-778A-4069-8EAA-0384F68F231D}">
       <text>
         <r>
           <rPr>
@@ -223,7 +368,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{006CA0A7-848C-4654-84E8-1EDEACFD0267}">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{4B74188F-39F2-45CF-AD8D-1FE0CF9F3BFE}">
       <text>
         <r>
           <rPr>
@@ -231,6 +376,54 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Het kan in dus in tekst beschreven worden (samen met andere informatie over volledigheid, juistheid en actualiteit wb de objecten van een objecttype). Alternatief is: in MIM kan dit specifieker aangekaart worden op het niveau van kenmerken. We zouden dit ook voor objecttypes kunnen doen, maar dit kan consequenties hebben bij transformaties (bv, zie in MIM: 6.4.9.15 transformatie: mogelijk geen waarde)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{097C8F23-BBA4-447C-A3ED-4A153DA8F751}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ook mogelijk via een nieuwe tagged value (?)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{216A7B36-531D-4F54-95FC-93933C23D997}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
           <t>Gabriella Wiersma:</t>
@@ -243,7 +436,55 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-wanneer dit afwijkt van de bronhouder voor het objecttype (het gaat om het opnemen van uitzonderingen, dus?)</t>
+Het gaat over verwijzingen naar documenten/luchtfoto's/plaatsbepalingspunten. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{392801EC-9BA4-4B8F-B297-0DE1AEFAF29F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Het vastleggen gebeurt op het niveu van de instanties. Echter kunnen we op informatiemodelniveau bv nog een lijst met mogelijke waardes vastleggen (afhankelijk van hoe wordt omgegaan met wijzigingen op attribuutniveau)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{F4611A28-234A-48E7-BE0E-7E1F518FD6F9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+mogelijk via een nieuwe tagged value (?)</t>
         </r>
       </text>
     </comment>
@@ -269,6 +510,234 @@
           <t xml:space="preserve">
 Of deze functionaliteit wel gewenst is (makkelijk het IM kunnen aanpassen voor dit doel), is een vraag voor de Architectuur
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{6E2A199E-3427-4B2D-B64B-8DF34CD1F0FC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+of mim tagged values voldoende zijn hangt af van de mate van kwaliteitsbeschrijving die nodig is voor de SOR. Dit moet nog duidelijk worden.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{6491E7DD-F871-4084-A87F-8C6101B6A02B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+actualiteit + wijze van inwinning kunnen we beschrijven met mim:kwaliteit, precisie mogelijk met mim:lengte</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C25" authorId="0" shapeId="0" xr:uid="{E716265D-5950-4923-9AEA-4E6F45599F9A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mogelijk nodig, afhankelijk van keuzes voor patronen wb historie/metadata op attribuutniveau</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{BB6AE970-D84C-4BE2-AAFA-CCBB8D3717DD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Gabriella Wiersma:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dit staat wellicht in de EMSO maar we willen het NIET hier behandelen - historie en levensfase aspecten behandelen we al in een apart traject.
+*"Concreet" betekent dat de beschrijving eigenlijk een invulling betreft van de eis</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C26" authorId="0" shapeId="0" xr:uid="{58DA8577-6D9E-4CBE-8234-D3C508A9D8AE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hier wordt gesproken over meta-informatie van elk ''object'': het lijkt te gaan om de inwinning, het lijkt op een eis aan bronhouders. Vanuit de modellering kunnen we dit eventueel interpreteren als ''in het model leggen we vast dat historie kan worden geraadpleegd voor bepaalde kenmerken van bepaalde objecttypes" - Dit kan met MIM.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E26" authorId="0" shapeId="0" xr:uid="{754BD94D-B73B-4031-A0E5-788C48BA439D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Indicatie historie op het niveau van kenmerken (attributen) van een objecttype, op conceptueel niveau</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E27" authorId="0" shapeId="0" xr:uid="{4B39564C-3E05-48A7-905D-79D14CEDC95F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+verhouding tussen herkomst in MIM, herkomst in begrippenkader (dcterms:source) en relatie modelelement-definitie-begrip vereist meer aandacht</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E28" authorId="0" shapeId="0" xr:uid="{FC1419B0-DB96-42F4-A98F-C31BDFFE3C45}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+verhouding tussen herkomst in MIM, herkomst in begrippenkader (dcterms:source) en relatie modelelement-definitie-begrip vereist meer aandacht</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{C2F7ABE4-1EAE-471B-AE23-ECCAF9627FEA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Als we dit ergens toepassen op logisch niveau, deze tagged value opnemen bij het typerende attribut</t>
         </r>
       </text>
     </comment>
@@ -307,7 +776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{31CBC20D-2EEF-41A9-98EB-3D7308C517C7}">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{CAE14932-1E12-44C2-8BF6-F63929A24EBD}">
       <text>
         <r>
           <rPr>
@@ -317,37 +786,21 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Gabriella Wiersma:
-Dit staat wellicht in de EMSO maar we willen het NIET hier behandelen - historie en levensfase aspecten behandelen we al in een apart traject
-</t>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ze zeggen geometrie, maar als het van toepassing is op alle geometrieen bedoelen ze misschien op dataset niveau? </t>
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{CAE14932-1E12-44C2-8BF6-F63929A24EBD}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Gabriella Wiersma:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Ze zeggen geometrie, maar als het van toepassing is op alle geometrieen bedoelen ze misschien op dataset niveau? </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{678C9498-0FBC-490C-82E7-CC3AB09EC30C}">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{678C9498-0FBC-490C-82E7-CC3AB09EC30C}">
       <text>
         <r>
           <rPr>
@@ -410,7 +863,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="170">
   <si>
     <t>Het gaat om metadata over informatieobjecten en hun gegevens</t>
   </si>
@@ -532,22 +985,13 @@
     <t>Beschrijving minimale eisen aan kwaliteit (nauwkeurigheid, actualiteit)</t>
   </si>
   <si>
-    <t>Vastleggen of planstatus relevant is</t>
-  </si>
-  <si>
     <t>Voor netwerken: de geometrie zal zich moeten bevinden binnen de contouren van de bijbehorende reele objecten</t>
   </si>
   <si>
     <t>Uit EMSO (in 2.4.4)</t>
   </si>
   <si>
-    <t>Historie/Levensfase</t>
-  </si>
-  <si>
     <t>Van elk object in de SOR wordt meta-informatie opgenomen over het ontstaansmoment en versie van het object</t>
-  </si>
-  <si>
-    <t>Uit EMSO (in 2.4.5)</t>
   </si>
   <si>
     <t>Minimale geometrietype die van toepassing is (2D, 2.5D, 3D)</t>
@@ -798,12 +1242,6 @@
     <t>Vastleggen of objecttype verplicht of optioneel is</t>
   </si>
   <si>
-    <t>Definitie van objecttype</t>
-  </si>
-  <si>
-    <t>Vastleggen actualiteitseis</t>
-  </si>
-  <si>
     <t>Definitie van attribuuttype</t>
   </si>
   <si>
@@ -865,20 +1303,167 @@
     <t>LI_ProcessStep.dateTime</t>
   </si>
   <si>
-    <t>ISO 19157</t>
-  </si>
-  <si>
     <t>Completeness</t>
   </si>
   <si>
     <t>Positional accuracy, temporal quality</t>
+  </si>
+  <si>
+    <t>Domein</t>
+  </si>
+  <si>
+    <t>Aanduiding van het functionele domein waartoe het informatiemodel behoort.</t>
+  </si>
+  <si>
+    <t>Model type</t>
+  </si>
+  <si>
+    <t>Uit 2.8.1.1 (verplicht)</t>
+  </si>
+  <si>
+    <t>Uit 2.8.1.2 (verplicht)</t>
+  </si>
+  <si>
+    <t>De beschrijving van de aard van het informatiemodel, hoe het geinterpreteerd moet worden. (conceptueel, logisch, technisch)</t>
+  </si>
+  <si>
+    <t>Relatiekeuze type</t>
+  </si>
+  <si>
+    <t>Aanduiding van een in MIM gedefinieerd alternatief voor een modelleringswijze, en welke keuze hierbij is gemaakt.</t>
+  </si>
+  <si>
+    <t>Uit 2.8.1.3 (verplicht)</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Versie MIM</t>
+  </si>
+  <si>
+    <t>De versie van de MIM specificatie die gebruikt is om het informatiemodel in uit te drukken.</t>
+  </si>
+  <si>
+    <t>Uit 2.8.1.4 (verplicht)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extensie MIM </t>
+  </si>
+  <si>
+    <t>De aanduiding van een extensie op MIM.</t>
+  </si>
+  <si>
+    <t>Uit 2.8.1.5 (optioneel)</t>
+  </si>
+  <si>
+    <t>Definitie van objecttype (naam, definitie, begrip)</t>
+  </si>
+  <si>
+    <t>In 2.8.2.1-2.8.2.7</t>
+  </si>
+  <si>
+    <t>Model (objecttype)</t>
+  </si>
+  <si>
+    <t>Model (dataset)</t>
+  </si>
+  <si>
+    <t>Model (kenmerk)</t>
+  </si>
+  <si>
+    <t>In 2.8.2.10</t>
+  </si>
+  <si>
+    <t>Uit EMSO (in 2.5.4)</t>
+  </si>
+  <si>
+    <t>Indicatie softtyping</t>
+  </si>
+  <si>
+    <t>Indicatie dat een attribuutsoort het objecttype waar het bijhoort classificeert in (sub)typen.</t>
+  </si>
+  <si>
+    <t>Uit 2.8.2.15</t>
+  </si>
+  <si>
+    <t>Onderbouwing van gegevens. Kan formeel zijn (in de vorm van een verwijzing naar vergunningen of besluiten), of technisch (verwijzing naar plaatsbepalingspunten, luchtfoto's, metingen of BIM-modellen).</t>
+  </si>
+  <si>
+    <t>Uit EMSO 3.4.1</t>
+  </si>
+  <si>
+    <t>Vastleggen van een reden van wijziging van een attribuutwaarde</t>
+  </si>
+  <si>
+    <t>Vastleggen van een reden van wijziging van een attribuutwaarde. Het is aan te bevelen om "reden van wijziging" vast te leggen aan de hand van te benoemen redenen.</t>
+  </si>
+  <si>
+    <t>Vastleggen of een bronverwijzing (naar bv vergunningen, plaatsbepalingspunten, etc) aan de orde is voor dit kenmerk</t>
+  </si>
+  <si>
+    <t>Uit EMSO 3.4.1 / 3.4.4</t>
+  </si>
+  <si>
+    <t>nvt</t>
+  </si>
+  <si>
+    <t>Historie/Levensfase (Concreet)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In het kader van de autorisatie kan per object vastgelegd worden wie de verantwoordelijke bronhouder is. Dat kan bijvoorbeeld de aanduiding zijn welke gemeente verantwoordelijk is voor het bijhouden van het betreffende object. </t>
+  </si>
+  <si>
+    <t>Vastleggen bronhouder(s): Het is mogelijk dat in het informatiemodel wordt gespecificeerd dat er verschillende (categorieën) bronhouders zijn voor één objecttype. De bronhouder is de partij die objecten kan opvoeren en afvoeren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vastleggen autorisatie gebruik: Als default zijn alle objecten in de SOR als open data voor iedereen beschikbaar. Uitzonderingen hierop worden in het informatiemodel expliciet benoemd. </t>
+  </si>
+  <si>
+    <t>*invulling nodig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2.8.2.16 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vastleggen of planstatus relevant is (relevant ontstaansmoment voor de SOR): Objecten worden in de SOR opgenomen op het moment dat deze volgens de voor het betreffende objecttype gedefinieerde criteria ontstaan </t>
+  </si>
+  <si>
+    <t>Objecttype/kenmerk</t>
+  </si>
+  <si>
+    <t>Voor elk objecttype is vastgelegd welke levensfasen in de vastlegging van een object worden onderscheiden.</t>
+  </si>
+  <si>
+    <t>Vastleggen actualiteitseis: gaat over binnen welke termijn (aantal dagen/maanden) na realisatie/ontstaan van een object, dit object beschikbaar moet zijn in de SOR</t>
+  </si>
+  <si>
+    <t>Zie diagram in 6.1.2 / 3.2.1 "populatie''</t>
+  </si>
+  <si>
+    <t>Zie diagram in 6.1.2 / 3.2.1 "kwaliteit''</t>
+  </si>
+  <si>
+    <t>Vastleggen autorisatie gebruik:  wanneer deze afwijken van de autorisatie voor het objecttype. Het is bijvoorbeeld mogelijk dat in de SOR voor een bepaald attribuut een andere bronhouder (attribuuthouder) wordt aangewezen.</t>
+  </si>
+  <si>
+    <t>*invulling nodig + betere definitie van kwaliteit</t>
+  </si>
+  <si>
+    <t>Zie diagram in 6.1.2 / 3.2.1 "kwaliteit''; In 2.8.2.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zie diagram in 6.1.2 / 3.2.1 "kwaliteit'' </t>
+  </si>
+  <si>
+    <t>In EMSO?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -936,8 +1521,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -956,6 +1547,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -970,7 +1567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -996,6 +1593,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1012,6 +1614,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1311,22 +1917,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1909998-A091-4F15-B6EE-594CF3A50443}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="79.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="9" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -1337,19 +1944,40 @@
         <v>9</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>31</v>
+        <v>169</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1359,22 +1987,28 @@
       <c r="C2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>152</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1382,13 +2016,16 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
+        <v>152</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
@@ -1396,13 +2033,16 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>152</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
@@ -1410,35 +2050,44 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
+        <v>152</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
       </c>
+      <c r="E8" t="s">
+        <v>152</v>
+      </c>
       <c r="F8" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
@@ -1446,21 +2095,27 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>152</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="E10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1470,94 +2125,115 @@
       <c r="C11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="D12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="4" t="s">
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>107</v>
-      </c>
       <c r="D15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>152</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C17" t="s">
-        <v>99</v>
+      <c r="C17" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="E17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>121</v>
+        <v>56</v>
+      </c>
+      <c r="E18" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
@@ -1565,60 +2241,107 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="72" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>101</v>
+      </c>
+      <c r="E20" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>23</v>
+      <c r="B21" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>100</v>
+      </c>
+      <c r="D21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
-        <v>108</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>109</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>111</v>
-      </c>
-      <c r="F22" t="s">
-        <v>122</v>
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
-        <v>108</v>
+      <c r="B23" t="s">
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="E23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="14"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -1627,254 +2350,486 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3201B4-AC03-4E42-9502-09F502A21EC6}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
+      <c r="C3" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>157</v>
+      </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
+      <c r="C4" s="5" t="s">
+        <v>156</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>157</v>
+      </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>101</v>
+      <c r="C5" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>157</v>
+      </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
-        <v>38</v>
+      <c r="C6" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>157</v>
+      </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
-        <v>100</v>
+      <c r="C7" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>157</v>
+      </c>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>40</v>
+      <c r="C8" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C9" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
       <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C11" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>157</v>
+      </c>
       <c r="B12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="E12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>157</v>
+      </c>
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
-        <v>15</v>
+      <c r="C13" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>157</v>
+      </c>
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>166</v>
+      </c>
       <c r="B15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>167</v>
       </c>
       <c r="F15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>157</v>
+      </c>
       <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>157</v>
+      </c>
       <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>157</v>
+      </c>
       <c r="B18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C18" t="s">
-        <v>46</v>
+      <c r="C18" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" t="s">
+        <v>142</v>
+      </c>
+      <c r="E26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C19" t="s">
-        <v>103</v>
-      </c>
-      <c r="D19" t="s">
-        <v>61</v>
+      <c r="C27" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E29" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A20:E20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68CBA22-1ADA-494E-ABF5-6F9224856F94}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1911,6 +2866,12 @@
       </c>
       <c r="C2"/>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1922,7 +2883,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1930,6 +2891,7 @@
     <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="111.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1968,83 +2930,83 @@
         <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
         <v>44</v>
-      </c>
-      <c r="D4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="D6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="D7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>160</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>58</v>
+      <c r="C8" s="17" t="s">
+        <v>161</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2057,15 +3019,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABB184E-209E-4173-AFD2-9160777FEF28}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:L1"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.88671875" customWidth="1"/>
     <col min="7" max="7" width="19.109375" customWidth="1"/>
@@ -2076,34 +3038,34 @@
   <sheetData>
     <row r="1" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -2111,37 +3073,37 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
         <v>64</v>
       </c>
-      <c r="C2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" t="s">
-        <v>67</v>
-      </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -2152,34 +3114,34 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="K3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2190,34 +3152,34 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2241,28 +3203,28 @@
   <sheetData>
     <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2272,132 +3234,132 @@
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update metadata taken verdeling
</commit_message>
<xml_diff>
--- a/issues/60-metadata/inventarisatie_metadata_sor.xlsx
+++ b/issues/60-metadata/inventarisatie_metadata_sor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.wiersma\Documents\disgeo-imsor\issues\60-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96B50DB-EB11-4B1B-A120-D1D6898D40CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209BCA27-8617-40DC-A985-EB1799D51052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-564" yWindow="276" windowWidth="11328" windowHeight="12060" tabRatio="831" activeTab="1" xr2:uid="{A40E1B74-F992-4E2A-B94D-79E463DCBFBE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="831" firstSheet="1" activeTab="4" xr2:uid="{A40E1B74-F992-4E2A-B94D-79E463DCBFBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Instantieniveau" sheetId="3" r:id="rId1"/>
@@ -863,7 +863,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="174">
   <si>
     <t>Het gaat om metadata over informatieobjecten en hun gegevens</t>
   </si>
@@ -1457,6 +1457,19 @@
   </si>
   <si>
     <t>In EMSO?</t>
+  </si>
+  <si>
+    <t>ISO 191110</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>Gabriella</t>
+  </si>
+  <si>
+    <t>DCAT / Geo-DCAT-AP (DCAT 2)
+Data Catalog vocabulary</t>
   </si>
 </sst>
 </file>
@@ -1594,10 +1607,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1614,10 +1627,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1920,7 +1929,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2352,8 +2361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3201B4-AC03-4E42-9502-09F502A21EC6}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2689,13 +2698,13 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -3002,7 +3011,7 @@
       <c r="B8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>161</v>
       </c>
       <c r="D8" t="s">
@@ -3017,10 +3026,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABB184E-209E-4173-AFD2-9160777FEF28}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3028,6 +3037,7 @@
     <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.88671875" customWidth="1"/>
     <col min="7" max="7" width="19.109375" customWidth="1"/>
@@ -3036,7 +3046,7 @@
     <col min="10" max="11" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>62</v>
       </c>
@@ -3047,7 +3057,7 @@
         <v>72</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>66</v>
@@ -3067,8 +3077,11 @@
       <c r="L1" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3106,7 +3119,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3144,7 +3157,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3180,6 +3193,23 @@
       </c>
       <c r="L4" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F7" t="s">
+        <v>172</v>
+      </c>
+      <c r="H7" t="s">
+        <v>171</v>
+      </c>
+      <c r="J7" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mapping O&M en SSN toevoegen
hoort bij #60
</commit_message>
<xml_diff>
--- a/issues/60-metadata/inventarisatie_metadata_sor.xlsx
+++ b/issues/60-metadata/inventarisatie_metadata_sor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.wiersma\Documents\disgeo-imsor\issues\60-metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvandenbrink\Documents\github\disgeo-imsor\issues\60-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209BCA27-8617-40DC-A985-EB1799D51052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816140D1-02B3-4D0E-B297-1A3C4AD258B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="831" firstSheet="1" activeTab="4" xr2:uid="{A40E1B74-F992-4E2A-B94D-79E463DCBFBE}"/>
+    <workbookView xWindow="-38520" yWindow="-5400" windowWidth="38640" windowHeight="21240" tabRatio="831" xr2:uid="{A40E1B74-F992-4E2A-B94D-79E463DCBFBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Instantieniveau" sheetId="3" r:id="rId1"/>
@@ -212,7 +212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{1863180F-C074-4F49-9C4B-96B043FC5D6B}">
+    <comment ref="C24" authorId="0" shapeId="0" xr:uid="{1863180F-C074-4F49-9C4B-96B043FC5D6B}">
       <text>
         <r>
           <rPr>
@@ -863,7 +863,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="183">
   <si>
     <t>Het gaat om metadata over informatieobjecten en hun gegevens</t>
   </si>
@@ -1034,9 +1034,6 @@
   </si>
   <si>
     <t>Uit EMSO (in 3.4.1)</t>
-  </si>
-  <si>
-    <t>Beschrijving wijze van inwinning (precisie/nauwkeurigheid)</t>
   </si>
   <si>
     <t>Uit EMSO (in 3.4.2)</t>
@@ -1294,12 +1291,6 @@
 Geldt op dataset niveau maar kan op zich ok gebruikt worden op instantieniveau als het past.</t>
   </si>
   <si>
-    <t>DQ_AbsoluteExternalPositionalAccuracy.result</t>
-  </si>
-  <si>
-    <t>LI_SourceStep.processor &gt; CI_ResponsibleParty.organisationName</t>
-  </si>
-  <si>
     <t>LI_ProcessStep.dateTime</t>
   </si>
   <si>
@@ -1470,6 +1461,45 @@
   <si>
     <t>DCAT / Geo-DCAT-AP (DCAT 2)
 Data Catalog vocabulary</t>
+  </si>
+  <si>
+    <t>ObservingProcedure,
+Observer</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>precisie/nauwkeurigheid</t>
+  </si>
+  <si>
+    <t>SpatialSample/horizontalPositionalAccuracy</t>
+  </si>
+  <si>
+    <t>CI_ResponsibleParty</t>
+  </si>
+  <si>
+    <t>DQ_AbsoluteExternalPositionalAccuracy</t>
+  </si>
+  <si>
+    <t>phenomenonTime</t>
+  </si>
+  <si>
+    <t>ssn-system:Accuracy</t>
+  </si>
+  <si>
+    <t>sosa:phenomenonTime</t>
+  </si>
+  <si>
+    <t>sosa:usedProcedure</t>
+  </si>
+  <si>
+    <t>sosa:usedProcedure,
+ sosa:madeBySensor</t>
+  </si>
+  <si>
+    <t>sosa:isFeatureOfInterestOf
+ sosa:Observation</t>
   </si>
 </sst>
 </file>
@@ -1926,23 +1956,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1909998-A091-4F15-B6EE-594CF3A50443}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="79.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -1953,40 +1985,40 @@
         <v>9</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>32</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1997,27 +2029,39 @@
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="J2" t="s">
+        <v>149</v>
+      </c>
+      <c r="L2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="J3" t="s">
+        <v>149</v>
+      </c>
+      <c r="L3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -2025,16 +2069,22 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="J4" t="s">
+        <v>149</v>
+      </c>
+      <c r="L4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
@@ -2042,16 +2092,22 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="L5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
@@ -2059,30 +2115,42 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="J6" t="s">
+        <v>149</v>
+      </c>
+      <c r="L6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D7" t="s">
         <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="J7" t="s">
+        <v>149</v>
+      </c>
+      <c r="L7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>23</v>
       </c>
@@ -2090,13 +2158,19 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="J8" t="s">
+        <v>149</v>
+      </c>
+      <c r="L8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
@@ -2104,27 +2178,39 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="J9" t="s">
+        <v>149</v>
+      </c>
+      <c r="L9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="J10" t="s">
+        <v>149</v>
+      </c>
+      <c r="L10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2135,38 +2221,56 @@
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="J11" t="s">
+        <v>149</v>
+      </c>
+      <c r="L11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="J12" t="s">
+        <v>149</v>
+      </c>
+      <c r="L12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="J13" t="s">
+        <v>172</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
@@ -2177,13 +2281,19 @@
         <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="J14" t="s">
+        <v>149</v>
+      </c>
+      <c r="L14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
@@ -2194,160 +2304,247 @@
         <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="J15" t="s">
+        <v>149</v>
+      </c>
+      <c r="L15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
         <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>152</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>102</v>
+        <v>149</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" t="s">
+        <v>173</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
+        <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="L17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C18" t="s">
-        <v>25</v>
+      <c r="C18" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="J18" t="s">
+        <v>149</v>
+      </c>
+      <c r="L18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
         <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="J19" t="s">
+        <v>149</v>
+      </c>
+      <c r="L19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>152</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="J20" t="s">
+        <v>149</v>
+      </c>
+      <c r="L20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" t="s">
         <v>100</v>
       </c>
-      <c r="D21" t="s">
-        <v>101</v>
-      </c>
       <c r="E21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="J21" t="s">
+        <v>149</v>
+      </c>
+      <c r="L21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22" t="s">
+        <v>175</v>
+      </c>
+      <c r="J22" t="s">
+        <v>149</v>
+      </c>
+      <c r="L22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>30</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>56</v>
       </c>
-      <c r="E22" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="E23" t="s">
+        <v>149</v>
+      </c>
+      <c r="J23" t="s">
+        <v>149</v>
+      </c>
+      <c r="L23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>27</v>
       </c>
-      <c r="E23" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="4" t="s">
+      <c r="E24" t="s">
+        <v>149</v>
+      </c>
+      <c r="J24" t="s">
+        <v>149</v>
+      </c>
+      <c r="L24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" t="s">
         <v>103</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D25" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" t="s">
+        <v>114</v>
+      </c>
+      <c r="J25" t="s">
+        <v>177</v>
+      </c>
+      <c r="L25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
         <v>104</v>
       </c>
-      <c r="D24" t="s">
-        <v>106</v>
-      </c>
-      <c r="E24" t="s">
-        <v>152</v>
-      </c>
-      <c r="F24" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D26" t="s">
         <v>105</v>
       </c>
-      <c r="D25" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="14"/>
+      <c r="E26" t="s">
+        <v>149</v>
+      </c>
+      <c r="J26" t="s">
+        <v>149</v>
+      </c>
+      <c r="L26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -2361,22 +2558,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3201B4-AC03-4E42-9502-09F502A21EC6}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="92.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2387,38 +2585,38 @@
         <v>9</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>32</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="J1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>71</v>
-      </c>
       <c r="N1" s="8"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2429,43 +2627,43 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -2474,67 +2672,67 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
         <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D7" t="s">
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -2542,7 +2740,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2553,60 +2751,60 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E11" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>12</v>
@@ -2618,12 +2816,12 @@
         <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>12</v>
@@ -2632,18 +2830,18 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F15" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>12</v>
@@ -2652,15 +2850,15 @@
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>12</v>
@@ -2669,15 +2867,15 @@
         <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>12</v>
@@ -2689,138 +2887,138 @@
         <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B21" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" t="s">
         <v>120</v>
       </c>
-      <c r="C21" s="5" t="s">
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" t="s">
         <v>121</v>
       </c>
-      <c r="E21" t="s">
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" t="s">
         <v>125</v>
       </c>
-      <c r="E22" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C23" s="5" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="E23" t="s">
+      <c r="C24" s="5" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="15" t="s">
+      <c r="E24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="E25" t="s">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>138</v>
-      </c>
       <c r="B26" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E26" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>140</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E28" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E29" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2841,16 +3039,16 @@
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.33203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2869,16 +3067,16 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4"/>
     </row>
   </sheetData>
@@ -2891,19 +3089,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87312DF7-39D4-4F90-B695-A1AA5B2781D1}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="111.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="111.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2920,7 +3118,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2934,7 +3132,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2948,7 +3146,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -2962,7 +3160,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2976,7 +3174,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2990,7 +3188,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -3001,18 +3199,18 @@
         <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
         <v>41</v>
@@ -3028,98 +3226,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABB184E-209E-4173-AFD2-9160777FEF28}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5546875" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.88671875" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="11" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="11" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>71</v>
-      </c>
       <c r="M1" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
       <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
         <v>63</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" t="s">
         <v>63</v>
       </c>
-      <c r="G2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J2" t="s">
-        <v>64</v>
-      </c>
       <c r="K2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3127,37 +3325,37 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3165,51 +3363,51 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="L4" t="s">
         <v>63</v>
       </c>
-      <c r="J4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3222,174 +3420,174 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB73EB87-3B4E-46B8-9A64-F7FAE7AA310D}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+    <row r="31" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
+    <row r="35" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+    <row r="39" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update metadata inventarisatie (ISO 19157, ISO 19131, GeoDCAT)
</commit_message>
<xml_diff>
--- a/issues/60-metadata/inventarisatie_metadata_sor.xlsx
+++ b/issues/60-metadata/inventarisatie_metadata_sor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvandenbrink\Documents\github\disgeo-imsor\issues\60-metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.wiersma\Desktop\disgeo-imsor\issues\60-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816140D1-02B3-4D0E-B297-1A3C4AD258B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA285ED-8615-400A-A460-4B063ED13D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5400" windowWidth="38640" windowHeight="21240" tabRatio="831" xr2:uid="{A40E1B74-F992-4E2A-B94D-79E463DCBFBE}"/>
+    <workbookView xWindow="10980" yWindow="0" windowWidth="11148" windowHeight="11964" tabRatio="831" activeTab="1" xr2:uid="{A40E1B74-F992-4E2A-B94D-79E463DCBFBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Instantieniveau" sheetId="3" r:id="rId1"/>
@@ -295,6 +295,55 @@
         </r>
       </text>
     </comment>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{CDC9A57B-330B-4B03-84FA-6641588C4141}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Vanuit een dcat:Catalog/dcat:Dataset de relatie leggen naar een meerdere foaf:agents. Elke dcat:Catalog/dcat:Dataset moet dan wel betrekking hebben op één objecttype. 
+Over de ''categorieen'' van bronhouders: de typering van een foaf:agent wordt gecomuniceerd middels een skos:Concept. In de conceptscheme van dit concept zou je de bronhouders dus ook kunnen categoriseren.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{8E6DEDEF-B317-444C-AE2B-7182ADF15ACB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+textuele beschrijving is mogelijk</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E4" authorId="0" shapeId="0" xr:uid="{97262666-69BC-4EF9-ACFE-5E4FC2F8F68D}">
       <text>
         <r>
@@ -319,6 +368,56 @@
         </r>
       </text>
     </comment>
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{6DFE97B5-75B7-4FD3-BD84-A507D869401C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Als de uitzonderingen op het niveau van objecttypes zijn (en deze zien we als dcat:Resources), du kun je accessRights gebruiken + INSPIRE codelijst/textuele uitleg over restricties.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{AC3E3E13-93B2-4BF7-98DB-C5F28BAE28D8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Je kunt ''restrictions'' beschrijven in de ''identification and purpose of data product'' sectie - je kunt echter geen scoping gebruiken, dus het is niet mogelijk om het structureel per objecttype te specificeren. 
+Los van authorisatie, zou je kunnen aangeven dat bepaalde objecttypes optioneel zijn, via bv:
+SpecificationScope.level = featuretype &gt; DataContentAndStructure.narrativeDescription</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E5" authorId="0" shapeId="0" xr:uid="{FFC75014-49E1-4551-B2B5-A6FD9D783318}">
       <text>
         <r>
@@ -340,6 +439,30 @@
           </rPr>
           <t xml:space="preserve">
 via mim:populatie tagged value (niet direct beschreven in MIM doc, wel in het diagram)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{D184F3F0-2B5F-4C34-A62A-E9824541E364}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Als het per objecttype gewenst is, dan zou je dit kunnen doen door elke collectie van bepaalde objecttype als dcat:Resource te zien. </t>
         </r>
       </text>
     </comment>
@@ -392,6 +515,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{C55FFCDF-3322-42E7-B7F1-7D8D683F4071}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In GeoDCAT wordt dqv:QualityMeasurement alleen gebruikt voor ruimtelijke resolutie; in DQV kun je het gebruiken om andere eisen mee te specificeren</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E7" authorId="0" shapeId="0" xr:uid="{097C8F23-BBA4-447C-A3ED-4A153DA8F751}">
       <text>
         <r>
@@ -416,6 +563,78 @@
         </r>
       </text>
     </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{9DBBE3E6-EF4F-4834-A217-66216A0EAD4A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+hiermee leg je de eis niet vast, maar kun je testen of in dataset aan zulke (conceptuele) eisen kan worden voldaan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{8AB37281-D19B-4661-853E-9ABEDC7C6E48}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In GeoDCAT wordt dqv:QualityMeasurement alleen gebruikt voor ruimtelijke resolutie; in DQV kun je het gebruiken om andere eisen mee te specificeren</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{ADDE8C23-BE9B-4FFC-BC86-93D90684A773}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In GeoDCAT wordt dqv:QualityMeasurement alleen gebruikt voor ruimtelijke resolutie; in DQV kun je het gebruiken om andere eisen mee te specificeren</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C11" authorId="0" shapeId="0" xr:uid="{216A7B36-531D-4F54-95FC-93933C23D997}">
       <text>
         <r>
@@ -440,6 +659,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{9A534120-D9EB-4A9F-BED5-14BA5027205D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+[...] conceptual consistency is used to ensure that the correct feature properties are present for each feature instance.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{B564FDA2-A0DF-4DBF-82E0-FC37BD4F5897}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+nvt, tenzij je elk kenmerk als een dcat:Resource wil zien</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C12" authorId="0" shapeId="0" xr:uid="{392801EC-9BA4-4B8F-B297-0DE1AEFAF29F}">
       <text>
         <r>
@@ -485,6 +752,30 @@
           </rPr>
           <t xml:space="preserve">
 mogelijk via een nieuwe tagged value (?)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{57ADE280-DF7E-47EF-BCBC-EDFD30E75CF0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Dan zou je dit attribuut als een apart dcat:Resource moeten zien,</t>
         </r>
       </text>
     </comment>
@@ -513,6 +804,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{A957D996-023E-4DA6-867C-443F745141DD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+nvt, tenzij je elk kenmerk als een dcat:Resource wil zien. Je zou de volledigheid dan via dct:description kunnen specificeren, of middels DQV.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A15" authorId="0" shapeId="0" xr:uid="{6E2A199E-3427-4B2D-B64B-8DF34CD1F0FC}">
       <text>
         <r>
@@ -558,6 +873,178 @@
           </rPr>
           <t xml:space="preserve">
 actualiteit + wijze van inwinning kunnen we beschrijven met mim:kwaliteit, precisie mogelijk met mim:lengte</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G15" authorId="0" shapeId="0" xr:uid="{C1602FA0-99EC-4D7D-ACE4-65316B8A4636}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+nvt, tenzij je elk kenmerk als een dcat:Resource wil zien. Dan zou je dqv:QualityMeasurement voor spatia/temporal resolution kunnen gebruiken voor nauwkeurigheid en dcat:frequency voor actualiteit.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{D2F288B2-C227-463D-845B-2ACD2BF6867D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Dataquality.dataquality.element = DQ_element (die van toepassing is, wss: DQ_PositionalAccuracy)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{85D72119-2A29-4D82-B957-A8B72F4C7C9A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+nvt, zelfs als je elk kenmerk als een dcat:Resource wil zien. Alsnog heb je dan geen manier om eisen aan de inwinning te specificeren (buiten dct:description)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{CFC1B5E0-61B9-472C-82F1-6C06BE634121}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+De DQ_elements die je nodig hebt zijn afhankelijk van het soort eis, de soorten ''minimale inspanningsverplichtingen''</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{138D6EE3-5A6C-4FAE-A9BC-214064927776}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+DQ_element onduidelijk, maar je kunt het onder de noemer van ''data quality'' specificeren. Zie data spec van INSPIRE buildings (op https://inspire.ec.europa.eu/Themes/126/2892), sectie 7.3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G21" authorId="0" shapeId="0" xr:uid="{F0934236-7A49-48E3-83A6-2BFABD46FD3A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+keyword voor tekst, theme wanneer het een skos:Concept is</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G24" authorId="0" shapeId="0" xr:uid="{E4B03242-EF1B-447C-AC72-9CF55CF46FB8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriella Wiersma:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Je zou MIM als een dct:Standard kunnen zien en daaraan versie info koppelen. Ex:
+&lt;SOR...&gt; a dcat:Dataset ;
+dct:conformsTo &lt;MIM&gt;.
+&lt;MIM&gt; dct:Standard ;
+owl:versionInfo ''x.1''.</t>
         </r>
       </text>
     </comment>
@@ -863,7 +1350,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="219">
   <si>
     <t>Het gaat om metadata over informatieobjecten en hun gegevens</t>
   </si>
@@ -1294,12 +1781,6 @@
     <t>LI_ProcessStep.dateTime</t>
   </si>
   <si>
-    <t>Completeness</t>
-  </si>
-  <si>
-    <t>Positional accuracy, temporal quality</t>
-  </si>
-  <si>
     <t>Domein</t>
   </si>
   <si>
@@ -1500,6 +1981,120 @@
   <si>
     <t>sosa:isFeatureOfInterestOf
  sosa:Observation</t>
+  </si>
+  <si>
+    <t>DQM_SourceReference / DQ_TemporalQuality</t>
+  </si>
+  <si>
+    <t>DQ_TemporalQuality</t>
+  </si>
+  <si>
+    <t>DQ_DescriptiveResult</t>
+  </si>
+  <si>
+    <t>DQM_SourceReference</t>
+  </si>
+  <si>
+    <t>DQ_EvaluationMethod.referenceDoc</t>
+  </si>
+  <si>
+    <t>DQ_PositionalAccuracy (bv: mean value of positional uncertainties)</t>
+  </si>
+  <si>
+    <t>nvt / dct:rightsHolder / dcat:qualifiedAttribution</t>
+  </si>
+  <si>
+    <t>SpecificationScope.level = featuretype &gt; MaintenanceOfTheData.description</t>
+  </si>
+  <si>
+    <t>dct:accessRights - RightsStatement</t>
+  </si>
+  <si>
+    <t>DQ_Completeness</t>
+  </si>
+  <si>
+    <t>dct:description / dqv:QualityMeasurement / dct:accrualPeriodicity /</t>
+  </si>
+  <si>
+    <t>SpecificationScope.level = featuretype &gt; DataContentAndStructure.narrativeDescription / Maintenance.maintenanceAndUpdateFrequency</t>
+  </si>
+  <si>
+    <t>DQ_CompletenessOmission</t>
+  </si>
+  <si>
+    <t>dct:description  / dqv:QualityMeasurement</t>
+  </si>
+  <si>
+    <t>SpecificationScope.level = featuretype &gt; DataContentAndStructure.narrativeDescription</t>
+  </si>
+  <si>
+    <t>DQ_ConceptualConsistency, DQ_DomainConsistency</t>
+  </si>
+  <si>
+    <t>dct:description / dqv:QualityMeasurement</t>
+  </si>
+  <si>
+    <t>SpecificationScope.level = featuretype &gt; DataCaptureAndProduction.inclusionCriteria</t>
+  </si>
+  <si>
+    <t>dqv:QualityMeasurement</t>
+  </si>
+  <si>
+    <t>SpecificationScope.level = featuretype &gt; DataCaptureAndProduction.inclusionCriteria / Maintenance.maintenanceAndUpdateFrequency</t>
+  </si>
+  <si>
+    <t>Opstellen/uitvoeren van quality reports, conform ISO 19157 (?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nvt  </t>
+  </si>
+  <si>
+    <t>SpecificationScope.level = attributeType &gt; DataContentAndStructure.narrativeDescription</t>
+  </si>
+  <si>
+    <t>nvt / dct:rightsHolder / dct:accessRights</t>
+  </si>
+  <si>
+    <t>SpecificationScope.level = attributetype &gt; MaintenanceOfTheData.description</t>
+  </si>
+  <si>
+    <t>SpecificationScope.level = attributetype &gt; DataContentAndStructure.narrativeDescription</t>
+  </si>
+  <si>
+    <t>DQ_PositionalAccuracy, DQ_TemporalQuality</t>
+  </si>
+  <si>
+    <t>SpecificationScope.level = attributetype &gt; DataQuality.dataquality</t>
+  </si>
+  <si>
+    <t>SpecificationScope.level = attributetype &gt; DataCaptureAndProduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nvt </t>
+  </si>
+  <si>
+    <t>DQ_ConceptualConsistency, DQ_Completeness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcat:keyword / dcat:theme </t>
+  </si>
+  <si>
+    <t>DataProductSpecification.term</t>
+  </si>
+  <si>
+    <t>dct:description</t>
+  </si>
+  <si>
+    <t>DataProductSpecification.overview</t>
+  </si>
+  <si>
+    <t>dct:conformsTo</t>
+  </si>
+  <si>
+    <t>DQ_ConceptualConsistency</t>
+  </si>
+  <si>
+    <t>SpecificationScope.level = dataset &gt; DataQuality.dataquality</t>
   </si>
 </sst>
 </file>
@@ -1571,7 +2166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1596,6 +2191,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1610,7 +2211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -1641,6 +2242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1958,23 +2560,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1909998-A091-4F15-B6EE-594CF3A50443}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="79.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -1985,7 +2587,7 @@
         <v>9</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>32</v>
@@ -2018,7 +2620,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -2029,39 +2631,48 @@
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
         <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>107</v>
       </c>
+      <c r="G3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I3" t="s">
+        <v>147</v>
+      </c>
       <c r="J3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -2072,19 +2683,28 @@
         <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>108</v>
       </c>
+      <c r="G4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I4" t="s">
+        <v>147</v>
+      </c>
       <c r="J4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
@@ -2095,19 +2715,25 @@
         <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>109</v>
       </c>
+      <c r="H5" t="s">
+        <v>147</v>
+      </c>
+      <c r="I5" t="s">
+        <v>147</v>
+      </c>
       <c r="J5" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
@@ -2118,16 +2744,25 @@
         <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="G6" t="s">
+        <v>181</v>
+      </c>
+      <c r="H6" t="s">
+        <v>147</v>
+      </c>
+      <c r="I6" t="s">
+        <v>147</v>
       </c>
       <c r="J6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
@@ -2138,19 +2773,28 @@
         <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>110</v>
       </c>
+      <c r="G7" t="s">
+        <v>182</v>
+      </c>
+      <c r="H7" t="s">
+        <v>147</v>
+      </c>
+      <c r="I7" t="s">
+        <v>147</v>
+      </c>
       <c r="J7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>23</v>
       </c>
@@ -2158,19 +2802,28 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>111</v>
       </c>
+      <c r="G8" t="s">
+        <v>147</v>
+      </c>
+      <c r="H8" t="s">
+        <v>147</v>
+      </c>
+      <c r="I8" t="s">
+        <v>147</v>
+      </c>
       <c r="J8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
@@ -2181,19 +2834,28 @@
         <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>112</v>
       </c>
+      <c r="G9" t="s">
+        <v>183</v>
+      </c>
+      <c r="H9" t="s">
+        <v>147</v>
+      </c>
+      <c r="I9" t="s">
+        <v>147</v>
+      </c>
       <c r="J9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
@@ -2201,16 +2863,22 @@
         <v>106</v>
       </c>
       <c r="E10" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="H10" t="s">
+        <v>147</v>
+      </c>
+      <c r="I10" t="s">
+        <v>147</v>
       </c>
       <c r="J10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2221,56 +2889,77 @@
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="G11" t="s">
+        <v>184</v>
       </c>
       <c r="J11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="G12" t="s">
+        <v>147</v>
+      </c>
+      <c r="H12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I12" t="s">
+        <v>147</v>
       </c>
       <c r="J12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E13" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="G13" t="s">
+        <v>185</v>
+      </c>
+      <c r="H13" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" t="s">
+        <v>147</v>
       </c>
       <c r="J13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
@@ -2281,19 +2970,28 @@
         <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>107</v>
       </c>
+      <c r="G14" t="s">
+        <v>147</v>
+      </c>
+      <c r="H14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I14" t="s">
+        <v>147</v>
+      </c>
       <c r="J14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
@@ -2304,19 +3002,28 @@
         <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>108</v>
       </c>
+      <c r="G15" t="s">
+        <v>147</v>
+      </c>
+      <c r="H15" t="s">
+        <v>147</v>
+      </c>
+      <c r="I15" t="s">
+        <v>147</v>
+      </c>
       <c r="J15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>22</v>
       </c>
@@ -2327,37 +3034,55 @@
         <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="G16" t="s">
+        <v>186</v>
+      </c>
+      <c r="H16" t="s">
+        <v>147</v>
+      </c>
+      <c r="I16" t="s">
+        <v>147</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="C17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D17" t="s">
         <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F17" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G17" t="s">
+        <v>147</v>
+      </c>
+      <c r="H17" t="s">
+        <v>147</v>
+      </c>
+      <c r="I17" t="s">
+        <v>147</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="L17" t="s">
         <v>176</v>
       </c>
-      <c r="J17" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="L17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
         <v>22</v>
       </c>
@@ -2368,16 +3093,25 @@
         <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="G18" t="s">
+        <v>181</v>
+      </c>
+      <c r="H18" t="s">
+        <v>147</v>
+      </c>
+      <c r="I18" t="s">
+        <v>147</v>
       </c>
       <c r="J18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>22</v>
       </c>
@@ -2388,16 +3122,25 @@
         <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="G19" t="s">
+        <v>182</v>
+      </c>
+      <c r="H19" t="s">
+        <v>147</v>
+      </c>
+      <c r="I19" t="s">
+        <v>147</v>
       </c>
       <c r="J19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>22</v>
       </c>
@@ -2408,16 +3151,25 @@
         <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="G20" t="s">
+        <v>147</v>
+      </c>
+      <c r="H20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I20" t="s">
+        <v>147</v>
       </c>
       <c r="J20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>22</v>
       </c>
@@ -2428,19 +3180,28 @@
         <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
+      </c>
+      <c r="G21" t="s">
+        <v>147</v>
+      </c>
+      <c r="H21" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" t="s">
+        <v>147</v>
       </c>
       <c r="J21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L21" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>22</v>
       </c>
@@ -2451,19 +3212,28 @@
         <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F22" t="s">
-        <v>175</v>
+        <v>173</v>
+      </c>
+      <c r="G22" t="s">
+        <v>147</v>
+      </c>
+      <c r="H22" t="s">
+        <v>147</v>
+      </c>
+      <c r="I22" t="s">
+        <v>147</v>
       </c>
       <c r="J22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L22" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>23</v>
       </c>
@@ -2474,16 +3244,25 @@
         <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="G23" t="s">
+        <v>183</v>
+      </c>
+      <c r="H23" t="s">
+        <v>147</v>
+      </c>
+      <c r="I23" t="s">
+        <v>147</v>
       </c>
       <c r="J23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L23" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -2491,16 +3270,25 @@
         <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="G24" t="s">
+        <v>182</v>
+      </c>
+      <c r="H24" t="s">
+        <v>147</v>
+      </c>
+      <c r="I24" t="s">
+        <v>147</v>
       </c>
       <c r="J24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L24" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>102</v>
       </c>
@@ -2511,19 +3299,28 @@
         <v>105</v>
       </c>
       <c r="E25" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F25" t="s">
         <v>114</v>
       </c>
+      <c r="G25" t="s">
+        <v>182</v>
+      </c>
+      <c r="H25" t="s">
+        <v>147</v>
+      </c>
+      <c r="I25" t="s">
+        <v>147</v>
+      </c>
       <c r="J25" t="s">
+        <v>175</v>
+      </c>
+      <c r="L25" t="s">
         <v>177</v>
       </c>
-      <c r="L25" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" s="4" t="s">
         <v>102</v>
       </c>
@@ -2534,16 +3331,16 @@
         <v>105</v>
       </c>
       <c r="E26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L26" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="14"/>
     </row>
   </sheetData>
@@ -2558,23 +3355,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3201B4-AC03-4E42-9502-09F502A21EC6}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="92.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2585,7 +3382,7 @@
         <v>9</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>32</v>
@@ -2616,7 +3413,7 @@
       </c>
       <c r="N1" s="8"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2627,43 +3424,73 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s">
         <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="F3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I3" t="s">
+        <v>147</v>
+      </c>
+      <c r="K3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
         <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="F4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I4" t="s">
+        <v>147</v>
+      </c>
+      <c r="K4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -2675,15 +3502,27 @@
         <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="G5" t="s">
+        <v>191</v>
+      </c>
+      <c r="H5" t="s">
+        <v>192</v>
+      </c>
+      <c r="I5" t="s">
+        <v>147</v>
+      </c>
+      <c r="K5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
@@ -2695,52 +3534,106 @@
         <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="F6" t="s">
+        <v>193</v>
+      </c>
+      <c r="G6" t="s">
+        <v>194</v>
+      </c>
+      <c r="H6" t="s">
+        <v>195</v>
+      </c>
+      <c r="I6" t="s">
+        <v>147</v>
+      </c>
+      <c r="K6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D7" t="s">
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="F7" t="s">
+        <v>196</v>
+      </c>
+      <c r="G7" t="s">
+        <v>197</v>
+      </c>
+      <c r="H7" t="s">
+        <v>198</v>
+      </c>
+      <c r="I7" t="s">
+        <v>147</v>
+      </c>
+      <c r="K7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D8" t="s">
         <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="F8" t="s">
+        <v>147</v>
+      </c>
+      <c r="G8" t="s">
+        <v>199</v>
+      </c>
+      <c r="H8" t="s">
+        <v>200</v>
+      </c>
+      <c r="I8" t="s">
+        <v>147</v>
+      </c>
+      <c r="K8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F9" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="I9" t="s">
+        <v>147</v>
+      </c>
+      <c r="K9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2750,61 +3643,112 @@
       <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>147</v>
+      </c>
+      <c r="K10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="F11" t="s">
+        <v>196</v>
+      </c>
+      <c r="G11" t="s">
+        <v>202</v>
+      </c>
+      <c r="H11" t="s">
+        <v>203</v>
+      </c>
+      <c r="I11" t="s">
+        <v>147</v>
+      </c>
+      <c r="K11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="F12" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" t="s">
+        <v>147</v>
+      </c>
+      <c r="H12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I12" t="s">
+        <v>147</v>
+      </c>
+      <c r="K12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D13" t="s">
         <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="F13" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" t="s">
+        <v>204</v>
+      </c>
+      <c r="H13" t="s">
+        <v>205</v>
+      </c>
+      <c r="I13" t="s">
+        <v>147</v>
+      </c>
+      <c r="K13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>12</v>
@@ -2816,12 +3760,27 @@
         <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="F14" t="s">
+        <v>193</v>
+      </c>
+      <c r="G14" t="s">
+        <v>147</v>
+      </c>
+      <c r="H14" t="s">
+        <v>206</v>
+      </c>
+      <c r="I14" t="s">
+        <v>147</v>
+      </c>
+      <c r="K14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>12</v>
@@ -2833,15 +3792,27 @@
         <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="G15" t="s">
+        <v>147</v>
+      </c>
+      <c r="H15" t="s">
+        <v>208</v>
+      </c>
+      <c r="I15" t="s">
+        <v>147</v>
+      </c>
+      <c r="K15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>12</v>
@@ -2853,12 +3824,27 @@
         <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="F16" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" t="s">
+        <v>147</v>
+      </c>
+      <c r="H16" t="s">
+        <v>209</v>
+      </c>
+      <c r="I16" t="s">
+        <v>147</v>
+      </c>
+      <c r="K16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>12</v>
@@ -2870,12 +3856,27 @@
         <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="F17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G17" t="s">
+        <v>210</v>
+      </c>
+      <c r="H17" t="s">
+        <v>208</v>
+      </c>
+      <c r="I17" t="s">
+        <v>147</v>
+      </c>
+      <c r="K17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>12</v>
@@ -2887,115 +3888,247 @@
         <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="F18" t="s">
+        <v>211</v>
+      </c>
+      <c r="G18" t="s">
+        <v>147</v>
+      </c>
+      <c r="H18" t="s">
+        <v>208</v>
+      </c>
+      <c r="I18" t="s">
+        <v>147</v>
+      </c>
+      <c r="K18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="I19" t="s">
+        <v>147</v>
+      </c>
+      <c r="K19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>147</v>
+      </c>
+      <c r="K20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B21" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" t="s">
+        <v>147</v>
+      </c>
+      <c r="G21" t="s">
+        <v>212</v>
+      </c>
+      <c r="H21" t="s">
+        <v>213</v>
+      </c>
+      <c r="I21" t="s">
+        <v>147</v>
+      </c>
+      <c r="K21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C22" s="5" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
+      <c r="E22" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="F22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G22" t="s">
+        <v>214</v>
+      </c>
+      <c r="H22" t="s">
+        <v>215</v>
+      </c>
+      <c r="I22" t="s">
+        <v>147</v>
+      </c>
+      <c r="K22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E22" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="15" t="s">
+      <c r="E23" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G23" t="s">
+        <v>147</v>
+      </c>
+      <c r="H23" t="s">
+        <v>147</v>
+      </c>
+      <c r="I23" t="s">
+        <v>147</v>
+      </c>
+      <c r="K23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="15" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
+      <c r="C24" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="F24" t="s">
+        <v>147</v>
+      </c>
+      <c r="G24" t="s">
+        <v>216</v>
+      </c>
+      <c r="H24" t="s">
+        <v>147</v>
+      </c>
+      <c r="I24" t="s">
+        <v>147</v>
+      </c>
+      <c r="K24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="E24" t="s">
+      <c r="C25" s="5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="15" t="s">
+      <c r="E25" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E25" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>147</v>
+      </c>
+      <c r="G25" t="s">
+        <v>147</v>
+      </c>
+      <c r="H25" t="s">
+        <v>147</v>
+      </c>
+      <c r="I25" t="s">
+        <v>147</v>
+      </c>
+      <c r="K25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="F26" t="s">
+        <v>217</v>
+      </c>
+      <c r="G26" t="s">
+        <v>197</v>
+      </c>
+      <c r="H26" t="s">
+        <v>218</v>
+      </c>
+      <c r="I26" t="s">
+        <v>147</v>
+      </c>
+      <c r="K26" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D27" t="s">
         <v>57</v>
       </c>
       <c r="E27" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="F27" t="s">
+        <v>147</v>
+      </c>
+      <c r="G27" t="s">
+        <v>147</v>
+      </c>
+      <c r="H27" t="s">
+        <v>147</v>
+      </c>
+      <c r="I27" t="s">
+        <v>147</v>
+      </c>
+      <c r="K27" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>12</v>
@@ -3007,18 +4140,48 @@
         <v>57</v>
       </c>
       <c r="E28" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="F28" t="s">
+        <v>147</v>
+      </c>
+      <c r="G28" t="s">
+        <v>147</v>
+      </c>
+      <c r="H28" t="s">
+        <v>147</v>
+      </c>
+      <c r="I28" t="s">
+        <v>147</v>
+      </c>
+      <c r="K28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B29" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E29" t="s">
         <v>140</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="E29" t="s">
-        <v>142</v>
+      <c r="F29" t="s">
+        <v>147</v>
+      </c>
+      <c r="G29" t="s">
+        <v>147</v>
+      </c>
+      <c r="H29" t="s">
+        <v>147</v>
+      </c>
+      <c r="I29" t="s">
+        <v>147</v>
+      </c>
+      <c r="K29" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3039,16 +4202,16 @@
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3067,16 +4230,16 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C4"/>
     </row>
   </sheetData>
@@ -3093,15 +4256,15 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="111.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="111.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3118,7 +4281,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -3132,7 +4295,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3146,7 +4309,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -3160,7 +4323,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -3174,7 +4337,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3188,7 +4351,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -3202,15 +4365,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D8" t="s">
         <v>41</v>
@@ -3230,21 +4393,21 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="11" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="10" max="11" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>61</v>
       </c>
@@ -3255,7 +4418,7 @@
         <v>71</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>65</v>
@@ -3276,10 +4439,10 @@
         <v>70</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3317,7 +4480,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3355,7 +4518,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3393,21 +4556,21 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3424,168 +4587,168 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="76" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>61</v>
       </c>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
eis toevoegen over definitieve geometrie
</commit_message>
<xml_diff>
--- a/issues/60-metadata/inventarisatie_metadata_sor.xlsx
+++ b/issues/60-metadata/inventarisatie_metadata_sor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.wiersma\Desktop\disgeo-imsor\issues\60-metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvandenbrink\Documents\github\disgeo-imsor\issues\60-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E67A41-75F5-4B67-9986-CCDD38AADE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5104EBD9-0D29-4877-AEAC-4814209BF678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36" yWindow="240" windowWidth="11148" windowHeight="11964" tabRatio="831" activeTab="1" xr2:uid="{A40E1B74-F992-4E2A-B94D-79E463DCBFBE}"/>
+    <workbookView xWindow="-38520" yWindow="-5400" windowWidth="38640" windowHeight="21240" tabRatio="831" xr2:uid="{A40E1B74-F992-4E2A-B94D-79E463DCBFBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Instantieniveau" sheetId="3" r:id="rId1"/>
@@ -136,7 +136,7 @@
         <t>[Opmerkingenthread]
 U kunt deze opmerkingenthread lezen in uw versie van Excel. Eventuele wijzigingen aan de thread gaan echter verloren als het bestand wordt geopend in een nieuwere versie van Excel. Meer informatie: https://go.microsoft.com/fwlink/?linkid=870924
 Opmerking:
-    Niet zeker of ik PROV-O goed interpreteer. Deze property moet tussen 2 activiteiten gebruikt worden. De 2e activiteit is het controleren, maar wat is dan de eerste?</t>
+    Prov gaat vooral over: hoe is een informatieobject of gegeven tot stand gekomen. Wat je wel zou kunnen zeggen is dat door een prov:Activity "controle", een andere prov:Activity  "wijziging informatieobject" oid welke verbonden is met prov:wasInformedBy aan "controle" heeft geleid tot de nieuwe prov:Entity het informatieobject, of het gegeven</t>
       </text>
     </comment>
     <comment ref="C8" authorId="0" shapeId="0" xr:uid="{1966CE29-D1CC-4C92-8B77-715F87E2074D}">
@@ -1533,7 +1533,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="238">
   <si>
     <t>Het gaat om metadata over informatieobjecten en hun gegevens</t>
   </si>
@@ -1957,10 +1957,6 @@
     <t>LI_Source.description</t>
   </si>
   <si>
-    <t>ISO 19115
-Geldt op dataset niveau maar kan op zich ok gebruikt worden op instantieniveau als het past.</t>
-  </si>
-  <si>
     <t>LI_ProcessStep.dateTime</t>
   </si>
   <si>
@@ -2326,6 +2322,19 @@
   </si>
   <si>
     <t>check qSKOS quality assessment</t>
+  </si>
+  <si>
+    <t>Mate van definitief zijn van geometrie</t>
+  </si>
+  <si>
+    <t>Uit EMSO (in 5.3.1 en 6.2.1)</t>
+  </si>
+  <si>
+    <t>ISO 19115
+Geldt op dataset niveau maar kan op zich ook gebruikt worden op instantieniveau als het past.</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -2799,7 +2808,7 @@
     <text>Of dit past, is afhankeljik van hoe je 'verwijzing naar bron' invult. Met deze PROV property is het een verwijzing naar een Activity.</text>
   </threadedComment>
   <threadedComment ref="K6" dT="2021-07-16T08:18:52.20" personId="{AEB07A32-8143-4EB8-A909-F54C0A2C0225}" id="{7AD22F5E-3893-4BBC-A01D-16F5B0811DF1}">
-    <text>Niet zeker of ik PROV-O goed interpreteer. Deze property moet tussen 2 activiteiten gebruikt worden. De 2e activiteit is het controleren, maar wat is dan de eerste?</text>
+    <text>Prov gaat vooral over: hoe is een informatieobject of gegeven tot stand gekomen. Wat je wel zou kunnen zeggen is dat door een prov:Activity "controle", een andere prov:Activity  "wijziging informatieobject" oid welke verbonden is met prov:wasInformedBy aan "controle" heeft geleid tot de nieuwe prov:Entity het informatieobject, of het gegeven</text>
   </threadedComment>
   <threadedComment ref="K11" dT="2021-07-16T08:07:25.24" personId="{AEB07A32-8143-4EB8-A909-F54C0A2C0225}" id="{F4EA4602-8895-4E3A-AF4A-1B56D8CEE4D8}">
     <text>Of dit past, is afhankeljik van hoe je 'verwijzing naar bron' invult. Met deze PROV property is het een verwijzing naar een Activity.</text>
@@ -2823,25 +2832,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1909998-A091-4F15-B6EE-594CF3A50443}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="79.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" customWidth="1"/>
-    <col min="11" max="11" width="36.88671875" customWidth="1"/>
-    <col min="12" max="12" width="24.33203125" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="79.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="36.85546875" customWidth="1"/>
+    <col min="12" max="12" width="24.28515625" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="9" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -2852,13 +2861,13 @@
         <v>9</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>32</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>113</v>
+        <v>236</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>71</v>
@@ -2883,7 +2892,7 @@
       </c>
       <c r="N1" s="8"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -2894,57 +2903,57 @@
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" t="s">
         <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>107</v>
       </c>
       <c r="G3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
@@ -2955,31 +2964,31 @@
         <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>108</v>
       </c>
       <c r="G4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
@@ -2990,31 +2999,31 @@
         <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
@@ -3025,31 +3034,31 @@
         <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
@@ -3060,34 +3069,34 @@
         <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>110</v>
       </c>
       <c r="G7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>23</v>
       </c>
@@ -3095,31 +3104,31 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>111</v>
       </c>
       <c r="G8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
@@ -3130,31 +3139,31 @@
         <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>112</v>
       </c>
       <c r="G9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
@@ -3162,25 +3171,25 @@
         <v>106</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -3191,95 +3200,95 @@
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
@@ -3290,34 +3299,34 @@
         <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>107</v>
       </c>
       <c r="G14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
@@ -3328,31 +3337,31 @@
         <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>108</v>
       </c>
       <c r="G15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>22</v>
       </c>
@@ -3363,64 +3372,64 @@
         <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D17" t="s">
         <v>56</v>
       </c>
       <c r="E17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M17" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>22</v>
       </c>
@@ -3431,28 +3440,28 @@
         <v>100</v>
       </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>22</v>
       </c>
@@ -3463,31 +3472,31 @@
         <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M19" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>22</v>
       </c>
@@ -3498,31 +3507,31 @@
         <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M20" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>22</v>
       </c>
@@ -3533,34 +3542,34 @@
         <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>22</v>
       </c>
@@ -3571,34 +3580,34 @@
         <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M22" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>23</v>
       </c>
@@ -3609,28 +3618,28 @@
         <v>56</v>
       </c>
       <c r="E23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M23" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -3638,28 +3647,28 @@
         <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M24" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>102</v>
       </c>
@@ -3670,31 +3679,31 @@
         <v>105</v>
       </c>
       <c r="E25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J25" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M25" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>102</v>
       </c>
@@ -3705,19 +3714,57 @@
         <v>105</v>
       </c>
       <c r="E26" t="s">
-        <v>147</v>
+        <v>146</v>
+      </c>
+      <c r="I26" t="s">
+        <v>146</v>
       </c>
       <c r="J26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M26" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>234</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="E27" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" t="s">
+        <v>237</v>
+      </c>
+      <c r="G27" t="s">
+        <v>146</v>
+      </c>
+      <c r="H27" t="s">
+        <v>237</v>
+      </c>
+      <c r="I27" t="s">
+        <v>146</v>
+      </c>
+      <c r="J27" t="s">
+        <v>146</v>
+      </c>
+      <c r="L27" t="s">
+        <v>146</v>
+      </c>
+      <c r="M27" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="14"/>
     </row>
   </sheetData>
@@ -3732,24 +3779,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3201B4-AC03-4E42-9502-09F502A21EC6}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="92.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" customWidth="1"/>
-    <col min="8" max="8" width="36.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3760,7 +3807,7 @@
         <v>9</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>32</v>
@@ -3789,7 +3836,7 @@
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3800,85 +3847,85 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
         <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H3" t="s">
         <v>187</v>
       </c>
-      <c r="H3" t="s">
-        <v>188</v>
-      </c>
       <c r="I3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D4" t="s">
         <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -3890,33 +3937,33 @@
         <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" t="s">
         <v>190</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>191</v>
       </c>
-      <c r="H5" t="s">
-        <v>192</v>
-      </c>
       <c r="I5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
@@ -3928,107 +3975,107 @@
         <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G6" t="s">
         <v>193</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>194</v>
       </c>
-      <c r="H6" t="s">
-        <v>195</v>
-      </c>
       <c r="I6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D7" t="s">
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F7" t="s">
+        <v>195</v>
+      </c>
+      <c r="G7" t="s">
         <v>196</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>197</v>
       </c>
-      <c r="H7" t="s">
-        <v>198</v>
-      </c>
       <c r="I7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D8" t="s">
         <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G8" t="s">
+        <v>198</v>
+      </c>
+      <c r="H8" t="s">
         <v>199</v>
       </c>
-      <c r="H8" t="s">
-        <v>200</v>
-      </c>
       <c r="I8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -4036,22 +4083,22 @@
         <v>16</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -4062,135 +4109,135 @@
         <v>13</v>
       </c>
       <c r="I10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" t="s">
         <v>145</v>
       </c>
-      <c r="D11" t="s">
-        <v>146</v>
-      </c>
       <c r="E11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G11" t="s">
+        <v>201</v>
+      </c>
+      <c r="H11" t="s">
         <v>202</v>
       </c>
-      <c r="H11" t="s">
-        <v>203</v>
-      </c>
       <c r="I11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L11" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D13" t="s">
         <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G13" t="s">
+        <v>203</v>
+      </c>
+      <c r="H13" t="s">
         <v>204</v>
       </c>
-      <c r="H13" t="s">
-        <v>205</v>
-      </c>
       <c r="I13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L13" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>12</v>
@@ -4202,33 +4249,33 @@
         <v>56</v>
       </c>
       <c r="E14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>12</v>
@@ -4240,33 +4287,33 @@
         <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F15" t="s">
+        <v>206</v>
+      </c>
+      <c r="G15" t="s">
+        <v>146</v>
+      </c>
+      <c r="H15" t="s">
         <v>207</v>
       </c>
-      <c r="G15" t="s">
-        <v>147</v>
-      </c>
-      <c r="H15" t="s">
-        <v>208</v>
-      </c>
       <c r="I15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L15" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>12</v>
@@ -4278,33 +4325,33 @@
         <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L16" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>12</v>
@@ -4316,33 +4363,33 @@
         <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L17" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>12</v>
@@ -4354,301 +4401,301 @@
         <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L18" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K19" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
       <c r="I20" t="s">
+        <v>146</v>
+      </c>
+      <c r="J20" t="s">
+        <v>146</v>
+      </c>
+      <c r="K20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" t="s">
+        <v>146</v>
+      </c>
+      <c r="G21" t="s">
+        <v>211</v>
+      </c>
+      <c r="H21" t="s">
+        <v>212</v>
+      </c>
+      <c r="I21" t="s">
+        <v>146</v>
+      </c>
+      <c r="J21" t="s">
+        <v>146</v>
+      </c>
+      <c r="K21" t="s">
+        <v>146</v>
+      </c>
+      <c r="L21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" t="s">
+        <v>146</v>
+      </c>
+      <c r="G22" t="s">
+        <v>213</v>
+      </c>
+      <c r="H22" t="s">
+        <v>214</v>
+      </c>
+      <c r="I22" t="s">
+        <v>146</v>
+      </c>
+      <c r="J22" t="s">
+        <v>146</v>
+      </c>
+      <c r="K22" t="s">
+        <v>146</v>
+      </c>
+      <c r="L22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" t="s">
+        <v>146</v>
+      </c>
+      <c r="G23" t="s">
+        <v>146</v>
+      </c>
+      <c r="H23" t="s">
+        <v>146</v>
+      </c>
+      <c r="I23" t="s">
+        <v>146</v>
+      </c>
+      <c r="J23" t="s">
+        <v>146</v>
+      </c>
+      <c r="K23" t="s">
+        <v>146</v>
+      </c>
+      <c r="L23" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" t="s">
+        <v>146</v>
+      </c>
+      <c r="G24" t="s">
+        <v>215</v>
+      </c>
+      <c r="H24" t="s">
+        <v>146</v>
+      </c>
+      <c r="I24" t="s">
+        <v>146</v>
+      </c>
+      <c r="J24" t="s">
+        <v>146</v>
+      </c>
+      <c r="K24" t="s">
+        <v>146</v>
+      </c>
+      <c r="L24" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" t="s">
+        <v>146</v>
+      </c>
+      <c r="G25" t="s">
+        <v>146</v>
+      </c>
+      <c r="H25" t="s">
+        <v>146</v>
+      </c>
+      <c r="I25" t="s">
+        <v>146</v>
+      </c>
+      <c r="J25" t="s">
+        <v>146</v>
+      </c>
+      <c r="K25" t="s">
+        <v>146</v>
+      </c>
+      <c r="L25" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="J20" t="s">
-        <v>147</v>
-      </c>
-      <c r="K20" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E21" t="s">
-        <v>118</v>
-      </c>
-      <c r="F21" t="s">
-        <v>147</v>
-      </c>
-      <c r="G21" t="s">
-        <v>212</v>
-      </c>
-      <c r="H21" t="s">
-        <v>213</v>
-      </c>
-      <c r="I21" t="s">
-        <v>147</v>
-      </c>
-      <c r="J21" t="s">
-        <v>147</v>
-      </c>
-      <c r="K21" t="s">
-        <v>147</v>
-      </c>
-      <c r="L21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="E22" t="s">
-        <v>119</v>
-      </c>
-      <c r="F22" t="s">
-        <v>147</v>
-      </c>
-      <c r="G22" t="s">
-        <v>214</v>
-      </c>
-      <c r="H22" t="s">
-        <v>215</v>
-      </c>
-      <c r="I22" t="s">
-        <v>147</v>
-      </c>
-      <c r="J22" t="s">
-        <v>147</v>
-      </c>
-      <c r="K22" t="s">
-        <v>147</v>
-      </c>
-      <c r="L22" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E23" t="s">
-        <v>123</v>
-      </c>
-      <c r="F23" t="s">
-        <v>147</v>
-      </c>
-      <c r="G23" t="s">
-        <v>147</v>
-      </c>
-      <c r="H23" t="s">
-        <v>147</v>
-      </c>
-      <c r="I23" t="s">
-        <v>147</v>
-      </c>
-      <c r="J23" t="s">
-        <v>147</v>
-      </c>
-      <c r="K23" t="s">
-        <v>147</v>
-      </c>
-      <c r="L23" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E24" t="s">
-        <v>127</v>
-      </c>
-      <c r="F24" t="s">
-        <v>147</v>
-      </c>
-      <c r="G24" t="s">
-        <v>216</v>
-      </c>
-      <c r="H24" t="s">
-        <v>147</v>
-      </c>
-      <c r="I24" t="s">
-        <v>147</v>
-      </c>
-      <c r="J24" t="s">
-        <v>147</v>
-      </c>
-      <c r="K24" t="s">
-        <v>147</v>
-      </c>
-      <c r="L24" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E25" t="s">
-        <v>130</v>
-      </c>
-      <c r="F25" t="s">
-        <v>147</v>
-      </c>
-      <c r="G25" t="s">
-        <v>147</v>
-      </c>
-      <c r="H25" t="s">
-        <v>147</v>
-      </c>
-      <c r="I25" t="s">
-        <v>147</v>
-      </c>
-      <c r="J25" t="s">
-        <v>147</v>
-      </c>
-      <c r="K25" t="s">
-        <v>147</v>
-      </c>
-      <c r="L25" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>133</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F26" t="s">
+        <v>216</v>
+      </c>
+      <c r="G26" t="s">
+        <v>196</v>
+      </c>
+      <c r="H26" t="s">
         <v>217</v>
       </c>
-      <c r="G26" t="s">
-        <v>197</v>
-      </c>
-      <c r="H26" t="s">
-        <v>218</v>
-      </c>
       <c r="I26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L26" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D27" t="s">
         <v>57</v>
       </c>
       <c r="E27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L27" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>12</v>
@@ -4660,60 +4707,60 @@
         <v>57</v>
       </c>
       <c r="E28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L28" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="E29" t="s">
         <v>139</v>
       </c>
-      <c r="E29" t="s">
-        <v>140</v>
-      </c>
       <c r="F29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -4734,16 +4781,16 @@
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.33203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4762,16 +4809,16 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4"/>
     </row>
   </sheetData>
@@ -4788,15 +4835,15 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="111.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="111.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -4813,7 +4860,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -4827,7 +4874,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -4841,7 +4888,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -4855,7 +4902,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -4869,7 +4916,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -4883,7 +4930,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -4897,15 +4944,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8" t="s">
         <v>41</v>
@@ -4925,21 +4972,21 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5546875" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.88671875" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="11" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="11" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>61</v>
       </c>
@@ -4950,7 +4997,7 @@
         <v>71</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>65</v>
@@ -4971,10 +5018,10 @@
         <v>70</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -5012,7 +5059,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -5050,7 +5097,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -5088,21 +5135,21 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -5116,171 +5163,171 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>61</v>
       </c>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>94</v>
       </c>

</xml_diff>